<commit_message>
upgraded mac version to 1.10.0.0
</commit_message>
<xml_diff>
--- a/data/xlsx/lb.xlsx
+++ b/data/xlsx/lb.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736191BB-C611-794A-87A2-4B10B24AD813}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F739348-C6CC-C140-9BDD-23A015D702EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2180" windowWidth="19200" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2420" yWindow="6180" windowWidth="25600" windowHeight="14780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loadbalancers" sheetId="50" r:id="rId1"/>
     <sheet name="lblisteners" sheetId="53" r:id="rId2"/>
-    <sheet name="lbpolicies" sheetId="54" r:id="rId3"/>
-    <sheet name="lbrules" sheetId="55" r:id="rId4"/>
-    <sheet name="lbpools" sheetId="51" r:id="rId5"/>
-    <sheet name="lbmembers" sheetId="52" r:id="rId6"/>
+    <sheet name="lbpools" sheetId="51" r:id="rId3"/>
+    <sheet name="lbmembers" sheetId="52" r:id="rId4"/>
+    <sheet name="lbpolicies" sheetId="54" r:id="rId5"/>
+    <sheet name="lbrules" sheetId="55" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="63">
   <si>
     <t>*name</t>
   </si>
@@ -44,36 +44,12 @@
     <t>resource_group</t>
   </si>
   <si>
-    <t>create_timeout</t>
-  </si>
-  <si>
-    <t>delete_timeout</t>
-  </si>
-  <si>
-    <t>60m</t>
-  </si>
-  <si>
-    <t>update_timeout</t>
-  </si>
-  <si>
-    <t>vsi1</t>
-  </si>
-  <si>
-    <t>vsi2</t>
-  </si>
-  <si>
     <t>*subnets</t>
   </si>
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>lb1</t>
-  </si>
-  <si>
-    <t>public</t>
-  </si>
-  <si>
     <t>*lb</t>
   </si>
   <si>
@@ -98,18 +74,6 @@
     <t>session_persistence_type</t>
   </si>
   <si>
-    <t>session_persistence_cookie_name</t>
-  </si>
-  <si>
-    <t>lb1pool</t>
-  </si>
-  <si>
-    <t>round_robin</t>
-  </si>
-  <si>
-    <t>http</t>
-  </si>
-  <si>
     <t>*pool</t>
   </si>
   <si>
@@ -122,12 +86,6 @@
     <t>weight</t>
   </si>
   <si>
-    <t>lb1member1</t>
-  </si>
-  <si>
-    <t>lb1member2</t>
-  </si>
-  <si>
     <t>default_pool</t>
   </si>
   <si>
@@ -137,30 +95,15 @@
     <t>connection_limit</t>
   </si>
   <si>
-    <t>lb1listener</t>
-  </si>
-  <si>
-    <t>subnet1, subnet2</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>tags</t>
   </si>
   <si>
     <t>*listener</t>
   </si>
   <si>
-    <t>lb1policy</t>
-  </si>
-  <si>
     <t>*action</t>
   </si>
   <si>
-    <t>forward</t>
-  </si>
-  <si>
     <t>*priority</t>
   </si>
   <si>
@@ -188,22 +131,100 @@
     <t>*policy</t>
   </si>
   <si>
-    <t>10m</t>
-  </si>
-  <si>
     <t>health_monitor_port</t>
   </si>
   <si>
     <t>health_monitor_url</t>
   </si>
   <si>
-    <t>lb1rule</t>
-  </si>
-  <si>
-    <t>contains</t>
-  </si>
-  <si>
-    <t>header</t>
+    <t>*resource</t>
+  </si>
+  <si>
+    <t>webapptier-lb</t>
+  </si>
+  <si>
+    <t># Define webapptier LB listener</t>
+  </si>
+  <si>
+    <t>webapptier-lb-listener</t>
+  </si>
+  <si>
+    <t># Define webapptier LB pool</t>
+  </si>
+  <si>
+    <t>webapptier-lb-pool</t>
+  </si>
+  <si>
+    <t>var.webapptier-lb-algorithm</t>
+  </si>
+  <si>
+    <t>webapptier-lb-pool-member-zone1</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>length(ibm_is_instance.webappserver-zone1)</t>
+  </si>
+  <si>
+    <t>element(split("/", ibm_is_lb_pool.webapptier-lb-pool.id), 1)</t>
+  </si>
+  <si>
+    <t>element(ibm_is_instance.webappserver-zone1.*.primary_network_interface.0.primary_ipv4_address, count.index)</t>
+  </si>
+  <si>
+    <t>webapptier-lb-pool-member-zone2</t>
+  </si>
+  <si>
+    <t>element(ibm_is_instance.webappserver-zone2.*.primary_network_interface.0.primary_ipv4_address, count.index)</t>
+  </si>
+  <si>
+    <t>length(ibm_is_instance.webappserver-zone2)</t>
+  </si>
+  <si>
+    <t>ibm_is_lb.webapptier-lb.id</t>
+  </si>
+  <si>
+    <t>*file</t>
+  </si>
+  <si>
+    <t># Define webapptier LB in zone1 and zone2</t>
+  </si>
+  <si>
+    <t>"${var.vpc-name}-webapptier01-lb"</t>
+  </si>
+  <si>
+    <t>[ibm_is_subnet.webapptier-subnet-zone1.id, ibm_is_subnet.webapptier-subnet-zone2.id]</t>
+  </si>
+  <si>
+    <t>"public"</t>
+  </si>
+  <si>
+    <t>timeout.create</t>
+  </si>
+  <si>
+    <t>timeout.delete</t>
+  </si>
+  <si>
+    <t>lbaas.tf</t>
+  </si>
+  <si>
+    <t>"http"</t>
+  </si>
+  <si>
+    <t>timeout.update</t>
+  </si>
+  <si>
+    <t>"${var.vpc-name}-webapptier-lb-pool1"</t>
+  </si>
+  <si>
+    <t>"/"</t>
+  </si>
+  <si>
+    <t># Define webapptier LB pool members</t>
+  </si>
+  <si>
+    <t>ibm_resource_group.group.id</t>
   </si>
 </sst>
 </file>
@@ -254,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -262,12 +283,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.79998168889431442"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -283,12 +313,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
+  <dxfs count="50">
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -395,6 +428,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -405,6 +441,9 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -471,6 +510,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -523,6 +568,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -545,44 +596,94 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2ECE5DB1-D260-6E49-B492-4FB9F047A792}" name="Table3" displayName="Table3" ref="A1:G3" totalsRowShown="0" headerRowDxfId="43">
-  <autoFilter ref="A1:G3" xr:uid="{BF7B2943-D8B2-F141-A648-1F77292E609F}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7E74D83A-54A4-D149-81D3-7E89BF180D8D}" name="*name" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{C8993A1E-13ED-9646-B484-5C8D98EE5999}" name="*subnets" dataDxfId="41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2ECE5DB1-D260-6E49-B492-4FB9F047A792}" name="Table3" displayName="Table3" ref="A1:I6" totalsRowShown="0" headerRowDxfId="49">
+  <autoFilter ref="A1:I6" xr:uid="{BF7B2943-D8B2-F141-A648-1F77292E609F}"/>
+  <tableColumns count="9">
+    <tableColumn id="9" xr3:uid="{EF22B46C-EEC8-954B-9006-F5C934140BA4}" name="*file" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{14BCF91D-C69D-4A48-BAE6-6FE0CE708F39}" name="*resource" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{7E74D83A-54A4-D149-81D3-7E89BF180D8D}" name="*name" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{C8993A1E-13ED-9646-B484-5C8D98EE5999}" name="*subnets" dataDxfId="45"/>
     <tableColumn id="3" xr3:uid="{E05E3D1A-B4E0-144E-B4A0-2A74FB710BE1}" name="type"/>
     <tableColumn id="4" xr3:uid="{F53EAA06-1D92-0941-BD62-CFA25A63B0D9}" name="resource_group"/>
     <tableColumn id="7" xr3:uid="{2524A41E-F007-AE48-9710-277646E4A10F}" name="tags"/>
-    <tableColumn id="5" xr3:uid="{A420FD52-21F4-4942-82B5-3DC0138BED2A}" name="create_timeout"/>
-    <tableColumn id="6" xr3:uid="{5D32FBCD-73F2-AF48-BA9D-8F34A6D1A6E7}" name="delete_timeout"/>
+    <tableColumn id="5" xr3:uid="{A420FD52-21F4-4942-82B5-3DC0138BED2A}" name="timeout.create"/>
+    <tableColumn id="6" xr3:uid="{5D32FBCD-73F2-AF48-BA9D-8F34A6D1A6E7}" name="timeout.delete"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{94CB4938-803E-6A45-818C-239D4C2D3032}" name="Table14" displayName="Table14" ref="A1:J3" totalsRowShown="0" headerRowDxfId="40">
-  <autoFilter ref="A1:J3" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{E8A4E19C-7C80-BE4B-9D1A-EAF2138A1C8C}" name="*name"/>
-    <tableColumn id="2" xr3:uid="{58502468-21D1-1040-A10E-00FB04A9B10A}" name="*lb" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{36A4DC5F-3D00-1742-BF10-5AE11EE1736D}" name="*port" dataDxfId="38"/>
-    <tableColumn id="4" xr3:uid="{9FB55588-84BD-1745-A573-1D9D234CE5CF}" name="*protocol" dataDxfId="37"/>
-    <tableColumn id="5" xr3:uid="{243F434B-C4FC-9341-961C-5736FCAAFCB2}" name="default_pool" dataDxfId="36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{94CB4938-803E-6A45-818C-239D4C2D3032}" name="Table14" displayName="Table14" ref="A1:K6" totalsRowShown="0" headerRowDxfId="44">
+  <autoFilter ref="A1:K6" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{B213F9EA-EE5C-F141-83B8-5F805CCFF0B8}" name="*file"/>
+    <tableColumn id="11" xr3:uid="{BD2203B1-67E0-C748-8240-2DAB0412E863}" name="*resource"/>
+    <tableColumn id="2" xr3:uid="{58502468-21D1-1040-A10E-00FB04A9B10A}" name="*lb" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{36A4DC5F-3D00-1742-BF10-5AE11EE1736D}" name="*port" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{9FB55588-84BD-1745-A573-1D9D234CE5CF}" name="*protocol" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{243F434B-C4FC-9341-961C-5736FCAAFCB2}" name="default_pool" dataDxfId="40"/>
     <tableColumn id="6" xr3:uid="{E9C6B5E4-8F28-894E-AAF5-FD0372359A08}" name="certificate_instance"/>
     <tableColumn id="7" xr3:uid="{39FB495A-D741-DF4D-9CBB-33126FDB2888}" name="connection_limit"/>
-    <tableColumn id="8" xr3:uid="{B195A387-7290-6F4D-992D-FC6A35C6C037}" name="create_timeout"/>
-    <tableColumn id="9" xr3:uid="{D57D52D5-F852-574F-AC8C-D4F002C543A3}" name="update_timeout"/>
-    <tableColumn id="10" xr3:uid="{85A0B342-620E-6043-85AE-FEDAB97E276C}" name="delete_timeout"/>
+    <tableColumn id="8" xr3:uid="{B195A387-7290-6F4D-992D-FC6A35C6C037}" name="timeout.create"/>
+    <tableColumn id="9" xr3:uid="{D57D52D5-F852-574F-AC8C-D4F002C543A3}" name="timeout.update"/>
+    <tableColumn id="10" xr3:uid="{85A0B342-620E-6043-85AE-FEDAB97E276C}" name="timeout.delete"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E60FD6E6-8DD8-8245-8578-34024AB794A8}" name="Table142" displayName="Table142" ref="A1:H3" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="A1:H3" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{85162D83-2223-2743-94A8-CBB5DCABF5E2}" name="Table5" displayName="Table5" ref="A1:P6" totalsRowShown="0" headerRowDxfId="39">
+  <autoFilter ref="A1:P6" xr:uid="{BABC147B-328A-9E42-A692-B07DDF9AA10A}"/>
+  <tableColumns count="16">
+    <tableColumn id="16" xr3:uid="{878D88ED-76D1-9E45-AFBB-45E26283A42D}" name="*file" dataDxfId="38"/>
+    <tableColumn id="17" xr3:uid="{76B528BC-6979-CD40-AA48-F7EF2765CC75}" name="*resource" dataDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{1A08DB6B-DC44-4B4A-ACBB-35F1471E6D94}" name="*name" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{20D213A0-12B0-A448-93A2-6A4F802B619E}" name="*lb" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{C8D92085-C2A2-E94B-9427-75ADBDD22F85}" name="*algorithm" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{B3053301-5B4F-4F45-9DF1-DA16E8095157}" name="*protocol" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{7C332576-C537-4248-9FF0-2F9304672F27}" name="*health_delay" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{510D5DA4-96D6-9949-8E0A-ACCD7802CF77}" name="*health_retries" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{FADE0027-F404-2A4B-B748-0B5DED401559}" name="*health_timeout" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{48E221A6-8A70-8F49-9024-3BB8C6AB4DA4}" name="*health_type" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{DFCC5FFE-E582-F04E-A8A9-916B566859A5}" name="health_monitor_url" dataDxfId="28" dataCellStyle="Hyperlink"/>
+    <tableColumn id="15" xr3:uid="{FDF5BBAA-A030-0249-B742-785E3947CFDE}" name="health_monitor_port" dataDxfId="27" dataCellStyle="Hyperlink"/>
+    <tableColumn id="10" xr3:uid="{4A2772BB-820B-5A45-8BFB-F7F0C1B6AB42}" name="session_persistence_type" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{A27FBA85-3106-504B-9F02-448FD69509DA}" name="timeout.create" dataDxfId="25"/>
+    <tableColumn id="12" xr3:uid="{D1C30DEA-49E6-3D49-9C7A-D48F6B55A9A5}" name="timeout.update" dataDxfId="24"/>
+    <tableColumn id="14" xr3:uid="{6B54822D-58A6-6944-8211-A034328AAF7F}" name="timeout.delete"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{398DB5A6-1B4D-6846-8DA7-E5AD59B6CE38}" name="Table13" displayName="Table13" ref="A1:K7" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:K7" xr:uid="{84D85FF3-D4A2-A145-9664-43C3D0B8D1F9}"/>
+  <tableColumns count="11">
+    <tableColumn id="11" xr3:uid="{28A3F32E-57F6-8842-B2B2-A04B774CDA50}" name="*file" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{057B1271-2391-7841-A672-9AD2C1910205}" name="*resource" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{F2654A05-284B-0140-951D-DB928685A88A}" name="*pool" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{6B716C5D-FF66-C746-8CFC-062268AAF158}" name="*lb" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{FD67A3F5-D75B-CB4B-A024-92F7CD45A782}" name="*port" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{DD77321C-9398-EE40-BFFA-ECD6F45DA631}" name="*target_address" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{6D9BEBF8-3CC8-4A46-B1C0-8CAEB4F85B2B}" name="weight" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{F8E3EE05-E616-E84F-99DB-97543EF6C5C8}" name="timeout.create" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{2CB92F37-5516-0349-A041-0758DAC69BB1}" name="timeout.update" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{C8275C9E-6CB9-D448-B533-095FDC0C8E0D}" name="timeout.delete" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{C52E3E2D-54DD-9446-B067-67A8B4C63FC4}" name="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E60FD6E6-8DD8-8245-8578-34024AB794A8}" name="Table142" displayName="Table142" ref="A1:J5" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A1:J5" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
+  <tableColumns count="10">
+    <tableColumn id="9" xr3:uid="{E289064D-9E30-6C4C-8CE3-2300AC9C55C4}" name="*file"/>
+    <tableColumn id="8" xr3:uid="{8F49C81B-5D52-C346-A10B-A5E168959794}" name="*resource"/>
     <tableColumn id="1" xr3:uid="{2FF8BFB2-91EE-A446-86F9-74CD2B7E4EAB}" name="*name"/>
     <tableColumn id="2" xr3:uid="{2D2B65B1-D705-9545-9296-FDE0CA8FE849}" name="*lb" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{953F377D-3690-9F49-A2D7-13E4CAED4CFD}" name="*listener" dataDxfId="10"/>
@@ -596,63 +697,22 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB510EA5-FA28-F942-B096-4AD8DC157ED6}" name="Table1423" displayName="Table1423" ref="A1:K3" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:K3" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{EA0ED60E-D0DE-A34E-B60D-CD9A9972FEC9}" name="*name"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AB510EA5-FA28-F942-B096-4AD8DC157ED6}" name="Table1423" displayName="Table1423" ref="A1:L5" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:L5" xr:uid="{E37DA650-CD8A-9248-A324-C4E06B2EFAF3}"/>
+  <tableColumns count="12">
+    <tableColumn id="5" xr3:uid="{213A2C7B-26C4-134C-9946-55629CD5D7D8}" name="*file" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{EA0ED60E-D0DE-A34E-B60D-CD9A9972FEC9}" name="*resource"/>
     <tableColumn id="13" xr3:uid="{C22299AC-5863-9240-B1AA-3216DA25B339}" name="*lb"/>
     <tableColumn id="14" xr3:uid="{FA1F3712-5C50-2641-86F6-54A372B45FA7}" name="*listener"/>
     <tableColumn id="12" xr3:uid="{9746E68F-0349-A943-8FE6-2148B555D441}" name="*policy"/>
-    <tableColumn id="2" xr3:uid="{45833F8C-D38E-ED41-BC5F-DAE08C0A5977}" name="*condition" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{88A1F463-97BB-864F-BF22-27C4F4FB0251}" name="*type" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{40E5D8D5-E47A-EA4A-A9C4-DBCBB379F2A6}" name="*value" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{B42889C8-ED1D-4545-A953-28757B789A40}" name="*field" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{F5D58FE6-4D35-5647-8437-280C3798174F}" name="create_timeout" dataDxfId="2"/>
-    <tableColumn id="17" xr3:uid="{030D816A-4760-CD44-BD28-34039F851579}" name="update_timeout" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{663FF23A-35A0-084D-B859-8059110D2936}" name="delete_timeout"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{85162D83-2223-2743-94A8-CBB5DCABF5E2}" name="Table5" displayName="Table5" ref="A1:O3" totalsRowShown="0" headerRowDxfId="35">
-  <autoFilter ref="A1:O3" xr:uid="{BABC147B-328A-9E42-A692-B07DDF9AA10A}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{1A08DB6B-DC44-4B4A-ACBB-35F1471E6D94}" name="*name" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{20D213A0-12B0-A448-93A2-6A4F802B619E}" name="*lb" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{C8D92085-C2A2-E94B-9427-75ADBDD22F85}" name="*algorithm" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{B3053301-5B4F-4F45-9DF1-DA16E8095157}" name="*protocol" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{7C332576-C537-4248-9FF0-2F9304672F27}" name="*health_delay" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{510D5DA4-96D6-9949-8E0A-ACCD7802CF77}" name="*health_retries" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{FADE0027-F404-2A4B-B748-0B5DED401559}" name="*health_timeout" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{48E221A6-8A70-8F49-9024-3BB8C6AB4DA4}" name="*health_type" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{DFCC5FFE-E582-F04E-A8A9-916B566859A5}" name="health_monitor_url" dataDxfId="26" dataCellStyle="Hyperlink"/>
-    <tableColumn id="15" xr3:uid="{FDF5BBAA-A030-0249-B742-785E3947CFDE}" name="health_monitor_port" dataDxfId="0" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" xr3:uid="{4A2772BB-820B-5A45-8BFB-F7F0C1B6AB42}" name="session_persistence_type" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{8E803E34-ECD2-924E-A590-E2196A54A7B0}" name="session_persistence_cookie_name" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{A27FBA85-3106-504B-9F02-448FD69509DA}" name="create_timeout" dataDxfId="23"/>
-    <tableColumn id="12" xr3:uid="{D1C30DEA-49E6-3D49-9C7A-D48F6B55A9A5}" name="update_timeout" dataDxfId="22"/>
-    <tableColumn id="14" xr3:uid="{6B54822D-58A6-6944-8211-A034328AAF7F}" name="delete_timeout"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{398DB5A6-1B4D-6846-8DA7-E5AD59B6CE38}" name="Table13" displayName="Table13" ref="A1:I3" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="A1:I3" xr:uid="{84D85FF3-D4A2-A145-9664-43C3D0B8D1F9}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{057B1271-2391-7841-A672-9AD2C1910205}" name="*name" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{F2654A05-284B-0140-951D-DB928685A88A}" name="*pool" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{6B716C5D-FF66-C746-8CFC-062268AAF158}" name="*lb" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{FD67A3F5-D75B-CB4B-A024-92F7CD45A782}" name="*port" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{DD77321C-9398-EE40-BFFA-ECD6F45DA631}" name="*target_address" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{6D9BEBF8-3CC8-4A46-B1C0-8CAEB4F85B2B}" name="weight" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{F8E3EE05-E616-E84F-99DB-97543EF6C5C8}" name="create_timeout" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{2CB92F37-5516-0349-A041-0758DAC69BB1}" name="update_timeout" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{C52E3E2D-54DD-9446-B067-67A8B4C63FC4}" name="delete_timeout"/>
+    <tableColumn id="2" xr3:uid="{45833F8C-D38E-ED41-BC5F-DAE08C0A5977}" name="*condition" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{88A1F463-97BB-864F-BF22-27C4F4FB0251}" name="*type" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{40E5D8D5-E47A-EA4A-A9C4-DBCBB379F2A6}" name="*value" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{B42889C8-ED1D-4545-A953-28757B789A40}" name="*field" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{F5D58FE6-4D35-5647-8437-280C3798174F}" name="timeout.create" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{030D816A-4760-CD44-BD28-34039F851579}" name="timeout.update" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{663FF23A-35A0-084D-B859-8059110D2936}" name="timeout.delete"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -921,61 +981,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B909B7-5B7F-FE4A-8CD8-0D8F5B038E31}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="6" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -987,79 +1088,113 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711B9366-0593-C248-9411-B78B3C2D6CE0}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1">
-        <v>9080</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="1">
+        <v>80</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1070,68 +1205,195 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014ADAAB-5E2C-2345-B6AB-833E609C1DAB}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA16B708-803A-4C41-87F9-C6AEEBD9524B}">
+  <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="22.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1142,89 +1404,82 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717A1372-1645-6F46-82FB-B4CB472DCF87}">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F060F451-DD45-A340-881E-50BF9BBCCEF3}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="8" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="90.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
+      <c r="A1" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1233,8 +1488,86 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="1">
+        <v>80</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="1">
+        <v>80</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1243,235 +1576,86 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA16B708-803A-4C41-87F9-C6AEEBD9524B}">
-  <dimension ref="A1:O3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{014ADAAB-5E2C-2345-B6AB-833E609C1DAB}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="16.5" customWidth="1"/>
-    <col min="9" max="10" width="20.83203125" customWidth="1"/>
-    <col min="11" max="12" width="30.83203125" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="1">
-        <v>60</v>
-      </c>
-      <c r="F2" s="1">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>30</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="I1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="http://www.ibm.com" xr:uid="{1B7317C9-FBA6-3346-BFCE-62E83B3BCF09}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F060F451-DD45-A340-881E-50BF9BBCCEF3}">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1">
-        <v>8080</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1">
-        <v>60</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8080</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1">
-        <v>60</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>4</v>
-      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1479,4 +1663,112 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{717A1372-1645-6F46-82FB-B4CB472DCF87}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>